<commit_message>
Updated SQL DB & SQL Table - 04042019/1150AM
</commit_message>
<xml_diff>
--- a/SQL Table.xlsx
+++ b/SQL Table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlfredYKH\Desktop\Login MVC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B740A6-14EA-4A4A-B772-283C78CDDF4B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50CA4943-92F1-4201-8E25-F9B5112FD7BD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25840" windowHeight="14027" xr2:uid="{17FAF049-5025-445C-A5E1-75C7B6E3F7F7}"/>
+    <workbookView xWindow="2897" yWindow="1981" windowWidth="17979" windowHeight="10505" xr2:uid="{17FAF049-5025-445C-A5E1-75C7B6E3F7F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="68">
   <si>
     <t>Purchase</t>
   </si>
@@ -156,12 +156,6 @@
     <t>kelvin</t>
   </si>
   <si>
-    <t>URL</t>
-  </si>
-  <si>
-    <t>https://bit.ly/2UbPkmS</t>
-  </si>
-  <si>
     <t>https://ewc.wy.edu/wp-content/uploads/2014/05/excel2013.jpg</t>
   </si>
   <si>
@@ -205,13 +199,49 @@
   </si>
   <si>
     <t>fd472eb2-567a-11e9-8647-d663bd873d93</t>
+  </si>
+  <si>
+    <t>DownloadLink</t>
+  </si>
+  <si>
+    <t>ProductImage</t>
+  </si>
+  <si>
+    <t>https://www.windows1024.com/media/catalog/product/m/i/microsoft-powerpoint-2016.jpg</t>
+  </si>
+  <si>
+    <t>https://cdn2.macworld.co.uk/cmsdata/reviews/3612551/outlook_icon_thumb900_1-1.jpg</t>
+  </si>
+  <si>
+    <t>https://pbs.twimg.com/profile_images/876909882095550465/VZyK5jOu_400x400.jpg</t>
+  </si>
+  <si>
+    <t>https://www.sketchappsources.com/resources/source-image/microsoft-one-drive-logo.png</t>
+  </si>
+  <si>
+    <t>https://products.office.com/en-sg/word</t>
+  </si>
+  <si>
+    <t>https://products.office.com/en-sg/excel</t>
+  </si>
+  <si>
+    <t>https://products.office.com/en-sg/powerpoint</t>
+  </si>
+  <si>
+    <t>https://products.office.com/en-sg/onenote/digital-note-taking-app</t>
+  </si>
+  <si>
+    <t>https://products.office.com/en-sg/outlook/email-and-calendar-software-microsoft-outlook</t>
+  </si>
+  <si>
+    <t>https://products.office.com/en-sg/onedrive-for-business/online-cloud-storage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -223,6 +253,20 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -245,10 +289,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -256,8 +301,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -570,25 +621,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2CFC92D-5941-4115-BB42-AA978850DACF}">
-  <dimension ref="B2:N25"/>
+  <dimension ref="B2:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" topLeftCell="B9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31:G36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.35" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.23046875" defaultRowHeight="14.15" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="9.21875" style="1"/>
-    <col min="2" max="6" width="12.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="67.109375" style="1" customWidth="1"/>
-    <col min="8" max="9" width="12.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5546875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="73.77734375" style="1" customWidth="1"/>
-    <col min="12" max="18" width="12.6640625" style="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.21875" style="1"/>
+    <col min="1" max="1" width="9.23046875" style="1"/>
+    <col min="2" max="6" width="12.69140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="78" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.921875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.69140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="15.53515625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="13.3828125" style="1" customWidth="1"/>
+    <col min="12" max="18" width="12.69140625" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.23046875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B2" s="2" t="s">
         <v>24</v>
       </c>
@@ -598,14 +650,10 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="I2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-    </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -628,22 +676,16 @@
         <v>7</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="M3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B4" s="1">
         <v>1001</v>
       </c>
@@ -660,25 +702,19 @@
         <v>123</v>
       </c>
       <c r="I4" s="1">
-        <v>801</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>18</v>
+        <v>13452</v>
+      </c>
+      <c r="J4" s="1">
+        <v>1001</v>
+      </c>
+      <c r="K4" s="1">
+        <v>803</v>
       </c>
       <c r="L4" s="1">
-        <v>89</v>
-      </c>
-      <c r="M4" s="1">
-        <v>100</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B5" s="1">
         <v>1002</v>
       </c>
@@ -695,25 +731,19 @@
         <v>123</v>
       </c>
       <c r="I5" s="1">
-        <v>802</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>19</v>
+        <v>13452</v>
+      </c>
+      <c r="J5" s="1">
+        <v>1001</v>
+      </c>
+      <c r="K5" s="1">
+        <v>805</v>
       </c>
       <c r="L5" s="1">
-        <v>99</v>
-      </c>
-      <c r="M5" s="1">
-        <v>100</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B6" s="1">
         <v>1003</v>
       </c>
@@ -730,25 +760,19 @@
         <v>123</v>
       </c>
       <c r="I6" s="1">
-        <v>803</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>17</v>
+        <v>13453</v>
+      </c>
+      <c r="J6" s="1">
+        <v>1002</v>
+      </c>
+      <c r="K6" s="1">
+        <v>801</v>
       </c>
       <c r="L6" s="1">
-        <v>78</v>
-      </c>
-      <c r="M6" s="1">
-        <v>100</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B7" s="1">
         <v>1004</v>
       </c>
@@ -765,22 +789,19 @@
         <v>123</v>
       </c>
       <c r="I7" s="1">
-        <v>804</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>20</v>
+        <v>13453</v>
+      </c>
+      <c r="J7" s="1">
+        <v>1002</v>
+      </c>
+      <c r="K7" s="1">
+        <v>802</v>
       </c>
       <c r="L7" s="1">
-        <v>78</v>
-      </c>
-      <c r="M7" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B8" s="1">
         <v>1005</v>
       </c>
@@ -797,39 +818,47 @@
         <v>123</v>
       </c>
       <c r="I8" s="1">
-        <v>805</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>21</v>
+        <v>13454</v>
+      </c>
+      <c r="J8" s="1">
+        <v>1001</v>
+      </c>
+      <c r="K8" s="1">
+        <v>806</v>
       </c>
       <c r="L8" s="1">
-        <v>89</v>
-      </c>
-      <c r="M8" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.4">
       <c r="I9" s="1">
-        <v>806</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>22</v>
+        <v>13455</v>
+      </c>
+      <c r="J9" s="1">
+        <v>1003</v>
+      </c>
+      <c r="K9" s="1">
+        <v>802</v>
       </c>
       <c r="L9" s="1">
-        <v>58</v>
-      </c>
-      <c r="M9" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="I10" s="1">
+        <v>13455</v>
+      </c>
+      <c r="J10" s="1">
+        <v>1003</v>
+      </c>
+      <c r="K10" s="1">
+        <v>804</v>
+      </c>
+      <c r="L10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B12" s="2" t="s">
         <v>0</v>
       </c>
@@ -839,7 +868,7 @@
       <c r="F12" s="2"/>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B13" s="2" t="s">
         <v>1</v>
       </c>
@@ -862,7 +891,7 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B14" s="1">
         <v>90001</v>
       </c>
@@ -879,13 +908,10 @@
         <v>2</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B15" s="1">
         <v>90001</v>
       </c>
@@ -902,22 +928,10 @@
         <v>1</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B16" s="1">
         <v>90001</v>
       </c>
@@ -934,19 +948,10 @@
         <v>1</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I16" s="1">
-        <v>13452</v>
-      </c>
-      <c r="K16" s="1">
-        <v>803</v>
-      </c>
-      <c r="L16" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B17" s="1">
         <v>90001</v>
       </c>
@@ -963,19 +968,10 @@
         <v>1</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I17" s="1">
-        <v>13452</v>
-      </c>
-      <c r="K17" s="1">
-        <v>805</v>
-      </c>
-      <c r="L17" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B18" s="1">
         <v>90002</v>
       </c>
@@ -992,22 +988,10 @@
         <v>2</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I18" s="1">
-        <v>13453</v>
-      </c>
-      <c r="J18" s="1">
-        <v>1002</v>
-      </c>
-      <c r="K18" s="1">
-        <v>801</v>
-      </c>
-      <c r="L18" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B19" s="1">
         <v>90002</v>
       </c>
@@ -1024,22 +1008,10 @@
         <v>1</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I19" s="1">
-        <v>13453</v>
-      </c>
-      <c r="J19" s="1">
-        <v>1002</v>
-      </c>
-      <c r="K19" s="1">
-        <v>802</v>
-      </c>
-      <c r="L19" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B20" s="1">
         <v>90002</v>
       </c>
@@ -1056,22 +1028,10 @@
         <v>2</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="I20" s="1">
-        <v>13454</v>
-      </c>
-      <c r="J20" s="1">
-        <v>1001</v>
-      </c>
-      <c r="K20" s="1">
-        <v>806</v>
-      </c>
-      <c r="L20" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B21" s="1">
         <v>90003</v>
       </c>
@@ -1088,22 +1048,10 @@
         <v>1</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I21" s="1">
-        <v>13455</v>
-      </c>
-      <c r="J21" s="1">
-        <v>1003</v>
-      </c>
-      <c r="K21" s="1">
-        <v>802</v>
-      </c>
-      <c r="L21" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B22" s="1">
         <v>90004</v>
       </c>
@@ -1120,22 +1068,10 @@
         <v>1</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="I22" s="1">
-        <v>13455</v>
-      </c>
-      <c r="J22" s="1">
-        <v>1003</v>
-      </c>
-      <c r="K22" s="1">
-        <v>804</v>
-      </c>
-      <c r="L22" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B23" s="1">
         <v>90004</v>
       </c>
@@ -1152,10 +1088,10 @@
         <v>1</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B24" s="1">
         <v>90005</v>
       </c>
@@ -1172,10 +1108,10 @@
         <v>2</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B25" s="1">
         <v>90005</v>
       </c>
@@ -1192,11 +1128,168 @@
         <v>1</v>
       </c>
       <c r="G25" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B30" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" s="2" t="s">
         <v>57</v>
       </c>
+      <c r="G30" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B31" s="1">
+        <v>801</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E31" s="1">
+        <v>89</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B32" s="1">
+        <v>802</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E32" s="1">
+        <v>99</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B33" s="1">
+        <v>803</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33" s="1">
+        <v>78</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B34" s="1">
+        <v>804</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E34" s="1">
+        <v>78</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B35" s="1">
+        <v>805</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E35" s="1">
+        <v>89</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B36" s="1">
+        <v>806</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E36" s="1">
+        <v>58</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>67</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G31" r:id="rId1" xr:uid="{19F37486-7FFE-42AC-9CDE-D5F796F2C42E}"/>
+    <hyperlink ref="G32" r:id="rId2" xr:uid="{DD8A4D15-ED83-4334-A2E7-27B9CE1CD140}"/>
+    <hyperlink ref="G33" r:id="rId3" xr:uid="{B59CD889-9BA4-469D-A2AC-36EE4EF46F6B}"/>
+    <hyperlink ref="G35" r:id="rId4" xr:uid="{2D086B96-121B-4DA1-B4D0-4FAFD5E5AE32}"/>
+    <hyperlink ref="G34" r:id="rId5" xr:uid="{B86A1446-CC51-42A4-83A3-9F3983AC560E}"/>
+    <hyperlink ref="G36" r:id="rId6" xr:uid="{25E5C17E-3F01-44C3-BEE1-878E18C03675}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated SQL DB & SQL Table - 04042019/1327
</commit_message>
<xml_diff>
--- a/SQL Table.xlsx
+++ b/SQL Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlfredYKH\Desktop\Login MVC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50CA4943-92F1-4201-8E25-F9B5112FD7BD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD54CC6-D427-4317-B89D-1D184647A2B4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2897" yWindow="1981" windowWidth="17979" windowHeight="10505" xr2:uid="{17FAF049-5025-445C-A5E1-75C7B6E3F7F7}"/>
+    <workbookView xWindow="2614" yWindow="549" windowWidth="20068" windowHeight="10505" xr2:uid="{17FAF049-5025-445C-A5E1-75C7B6E3F7F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -293,7 +293,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -305,7 +305,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -623,8 +622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2CFC92D-5941-4115-BB42-AA978850DACF}">
   <dimension ref="B2:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31:G36"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4:L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23046875" defaultRowHeight="14.15" x14ac:dyDescent="0.4"/>
@@ -702,7 +701,7 @@
         <v>123</v>
       </c>
       <c r="I4" s="1">
-        <v>13452</v>
+        <v>50001</v>
       </c>
       <c r="J4" s="1">
         <v>1001</v>
@@ -731,7 +730,7 @@
         <v>123</v>
       </c>
       <c r="I5" s="1">
-        <v>13452</v>
+        <v>50002</v>
       </c>
       <c r="J5" s="1">
         <v>1001</v>
@@ -760,7 +759,7 @@
         <v>123</v>
       </c>
       <c r="I6" s="1">
-        <v>13453</v>
+        <v>50003</v>
       </c>
       <c r="J6" s="1">
         <v>1002</v>
@@ -789,7 +788,7 @@
         <v>123</v>
       </c>
       <c r="I7" s="1">
-        <v>13453</v>
+        <v>50004</v>
       </c>
       <c r="J7" s="1">
         <v>1002</v>
@@ -818,7 +817,7 @@
         <v>123</v>
       </c>
       <c r="I8" s="1">
-        <v>13454</v>
+        <v>50005</v>
       </c>
       <c r="J8" s="1">
         <v>1001</v>
@@ -832,7 +831,7 @@
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.4">
       <c r="I9" s="1">
-        <v>13455</v>
+        <v>50006</v>
       </c>
       <c r="J9" s="1">
         <v>1003</v>
@@ -846,7 +845,7 @@
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.4">
       <c r="I10" s="1">
-        <v>13455</v>
+        <v>50007</v>
       </c>
       <c r="J10" s="1">
         <v>1003</v>
@@ -866,7 +865,6 @@
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
-      <c r="I12" s="2"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B13" s="2" t="s">
@@ -887,9 +885,6 @@
       <c r="G13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B14" s="1">
@@ -1213,7 +1208,7 @@
       <c r="E33" s="1">
         <v>78</v>
       </c>
-      <c r="F33" s="5" t="s">
+      <c r="F33" t="s">
         <v>58</v>
       </c>
       <c r="G33" s="3" t="s">
@@ -1233,7 +1228,7 @@
       <c r="E34" s="1">
         <v>78</v>
       </c>
-      <c r="F34" s="5" t="s">
+      <c r="F34" t="s">
         <v>59</v>
       </c>
       <c r="G34" s="3" t="s">
@@ -1253,7 +1248,7 @@
       <c r="E35" s="1">
         <v>89</v>
       </c>
-      <c r="F35" s="5" t="s">
+      <c r="F35" t="s">
         <v>60</v>
       </c>
       <c r="G35" s="3" t="s">
@@ -1273,7 +1268,7 @@
       <c r="E36" s="1">
         <v>58</v>
       </c>
-      <c r="F36" s="5" t="s">
+      <c r="F36" t="s">
         <v>61</v>
       </c>
       <c r="G36" s="3" t="s">

</xml_diff>